<commit_message>
//C = channelC in report, factor in rainfall file, direct Y
</commit_message>
<xml_diff>
--- a/auxfiles/coh.xlsx
+++ b/auxfiles/coh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A64D36-B3E2-4C74-B501-C2D5337A4747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52C4AF-2A95-4157-87C0-A66A38BE3F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B52F503B-D98B-4AC1-9EE3-A0A4342D3D10}"/>
   </bookViews>
@@ -1119,969 +1119,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6BEF-4246-A1DE-A86419227B09}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>s1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>19.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$4:$H$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>2.82</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.82</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.88</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.41</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1279999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.80571428571428572</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.70499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.62666666666666659</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.56399999999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.5127272727272727</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.43384615384615383</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.40285714285714286</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.376</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.35249999999999998</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.33176470588235291</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.3133333333333333</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.29684210526315785</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.28199999999999997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.26857142857142857</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.25636363636363635</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.2452173913043478</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.23499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.22559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.21692307692307691</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.20888888888888887</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.20142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.19448275862068964</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.188</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.18193548387096772</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.17624999999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.1709090909090909</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.16588235294117645</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.16114285714285714</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.15666666666666665</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.15243243243243243</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.14842105263157893</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.14461538461538462</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.14099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.13756097560975608</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.13428571428571429</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.13116279069767442</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.12818181818181817</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.12533333333333332</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-6BEF-4246-A1DE-A86419227B09}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>s2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>19.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$4:$I$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.666666666666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.5000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.2000000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.3333333333333335E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7142857142857144E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.2500000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8888888888888891E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.6000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.3636363636363636E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.1666666666666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8571428571428572E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.7333333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6250000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5294117647058824E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.4444444444444446E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.368421052631579E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.3000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.2380952380952381E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1818181818181818E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.1304347826086957E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0833333333333334E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.04E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.6296296296296303E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.285714285714286E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8.9655172413793099E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8.6666666666666663E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8.3870967741935479E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8.1250000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7.8787878787878792E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7.6470588235294122E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7.4285714285714285E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7.2222222222222228E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7.0270270270270272E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.842105263157895E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.5000000000000006E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.3414634146341468E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6.1904761904761907E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.0465116279069774E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.909090909090909E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.7777777777777784E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6BEF-4246-A1DE-A86419227B09}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>s2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>19.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$4:$I$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.666666666666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.5000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.2000000000000005E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.3333333333333335E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7142857142857144E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.2500000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8888888888888891E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.6000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.3636363636363636E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.1666666666666667E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8571428571428572E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.7333333333333333E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6250000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5294117647058824E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.4444444444444446E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.368421052631579E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.3000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.2380952380952381E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1818181818181818E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.1304347826086957E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0833333333333334E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.04E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.6296296296296303E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.285714285714286E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8.9655172413793099E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8.6666666666666663E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8.3870967741935479E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8.1250000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7.8787878787878792E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7.6470588235294122E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7.4285714285714285E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7.2222222222222228E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7.0270270270270272E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.842105263157895E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.5000000000000006E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.3414634146341468E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6.1904761904761907E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.0465116279069774E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.909090909090909E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.7777777777777784E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-6BEF-4246-A1DE-A86419227B09}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2913,10 +1950,10 @@
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3244,7 +2281,7 @@
   <dimension ref="D2:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
// mass balance for soil moisture, not working
</commit_message>
<xml_diff>
--- a/auxfiles/coh.xlsx
+++ b/auxfiles/coh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52C4AF-2A95-4157-87C0-A66A38BE3F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC8B91-6A6A-40F3-AAF2-32D66A7BDCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B52F503B-D98B-4AC1-9EE3-A0A4342D3D10}"/>
   </bookViews>
@@ -124,6 +124,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1260" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Detachment Efficiency Y</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -137,7 +162,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1260" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1137,6 +1162,7 @@
         <c:axId val="828310591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1154,6 +1180,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cohesion (kPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1176,7 +1257,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1199,6 +1280,7 @@
         <c:axId val="828311007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1238,7 +1320,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1280,7 +1362,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1327,7 +1409,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1050"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1950,10 +2032,10 @@
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2280,8 +2362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83643710-19E3-4F03-ABCD-6D1EB9E66F73}">
   <dimension ref="D2:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
// rewritten infiltrationdepthNew, some bug fixes and better link to percolation // max GW WH as prep for slope stability
</commit_message>
<xml_diff>
--- a/auxfiles/coh.xlsx
+++ b/auxfiles/coh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisem\auxfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC8B91-6A6A-40F3-AAF2-32D66A7BDCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E1B742-0502-40E2-A4E4-644AD8AE4037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B52F503B-D98B-4AC1-9EE3-A0A4342D3D10}"/>
   </bookViews>
@@ -2027,13 +2027,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
@@ -2363,7 +2363,7 @@
   <dimension ref="D2:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32:R32"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>